<commit_message>
Rieseguiti test per la nuova versione della checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ADLINGEGNERIAINFORMATICAXX/ADL/ARIA/2.99.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ADLINGEGNERIAINFORMATICAXX/ADL/ARIA/2.99.2/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\windev\Visual Studio 2019\[Migrato in GITLAB] Aria_V3\DOCUMENTAZIONE\ExternalResource\Fascicolo 2.0\_FSE 2\Accreditamento\Test\Aggiornamento_2025_12_05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\ACCREDITAMENTO\_2026_01_29\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83DC514-5926-4907-A05A-14CDCD892315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2300EE-5EF1-4CA9-A2A4-66F0D3ED8D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="504">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1725,175 +1725,190 @@
     <t>subject_application_version: 2.99.2</t>
   </si>
   <si>
-    <t>2025-12-05T16:35:54Z</t>
-  </si>
-  <si>
-    <t>e2768f51eb906092f8e4edd87a20072d</t>
-  </si>
-  <si>
-    <t>6506aa66-1c27-4e22-abcc-e215717942f0.9c717939a2a9a31bd0fab64231e9b14ca6e2d16958b3a06f57f0701c867c9b72.8063141458^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:33Z</t>
-  </si>
-  <si>
-    <t>09ab916e7746e206</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.31ced37a52^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Errore in fase di validazione</t>
   </si>
   <si>
     <t>Si procede alla sistemazione dei dati tramite intervento manuale e ritrasmissione del documento.</t>
   </si>
   <si>
-    <t>d197f47b70eba7ff</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.6bdc1863d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:32Z</t>
-  </si>
-  <si>
-    <t>25208d4f7b796b0b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.3e34dff0f8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:31Z</t>
-  </si>
-  <si>
-    <t>be3504aac0fb20c8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.9a48a92d83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:30Z</t>
-  </si>
-  <si>
-    <t>e29884afa05619c7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.50feefce79^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:29Z</t>
-  </si>
-  <si>
-    <t>543336d83925c306</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.97ceac3888^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:28Z</t>
-  </si>
-  <si>
-    <t>c36924a635994895</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.f31d149afa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:27Z</t>
-  </si>
-  <si>
-    <t>aca7727a64f49040</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.1d54b24921^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:26Z</t>
-  </si>
-  <si>
-    <t>4c1562d9561b6a3d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.5d22e8c57f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:24Z</t>
-  </si>
-  <si>
-    <t>bb39340a45617fd5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.b0fc2ea121^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:23Z</t>
-  </si>
-  <si>
-    <t>3460deaad52d28ae</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.5a1c496944^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>67de2aeb60be2535</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.aa41f563e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:22Z</t>
-  </si>
-  <si>
-    <t>9ec822a76cb5ae79</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.b5a7900c9e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:21Z</t>
-  </si>
-  <si>
-    <t>1fa8933a8e7d9750</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.7aa681b353^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:19Z</t>
-  </si>
-  <si>
-    <t>6cc5a2d1fdbaacf5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.80c4c95960^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:12:05Z</t>
-  </si>
-  <si>
-    <t>2024-07-11T16:11:35Z</t>
-  </si>
-  <si>
-    <t>6acc6d02bf982ac2</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2024-07-11T16:11:34Z</t>
-  </si>
-  <si>
-    <t>9b2143c4167370ca</t>
-  </si>
-  <si>
     <t>Si procede alla verifica della connettività tramite intervento manuale e successivamente viene ritrasmesso il documento.</t>
   </si>
   <si>
-    <t>Caso di test non presente al momento dell'accreditamento</t>
-  </si>
-  <si>
     <t>ADL</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:48Z</t>
+  </si>
+  <si>
+    <t>39223431b0f812b67dbef6fdcf421e8c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.aa05979868^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:50Z</t>
+  </si>
+  <si>
+    <t>4c7114ea5049fd0cbe5e4e5659ebf1b6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.4f5d3f18f3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>05e6a4b3ca053b74246c932f1553c2c1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.23ecd5f11a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:51Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.a2e4c0e3ac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b24f9cf32f8c250c63b4476658da2b0d</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:52Z</t>
+  </si>
+  <si>
+    <t>5d94c440acb848ad4fd2c4684495cb6d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.aed6d507c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:53Z</t>
+  </si>
+  <si>
+    <t>e585d53fc41affc777e569ac84f3df07</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.0043a95032^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a80ca470bd5c31200aca68a7286bbca4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.233e00a80e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:54Z</t>
+  </si>
+  <si>
+    <t>cec4ace9af4b7772579582f38a444c47</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.b0f5d5384f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:55Z</t>
+  </si>
+  <si>
+    <t>d6c06edd41ed1bd8ecb2ef54a797c2cb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.af543f4ff1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:56Z</t>
+  </si>
+  <si>
+    <t>fa7485490e2b3c497bda4648a9c1ae32</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.5305af7dcc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f3ef9a8754b2463aa39aedd5eab2f24c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.431f79ed35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:57Z</t>
+  </si>
+  <si>
+    <t>f3b73ab01eef4d38d2b0b51e3da5dce0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.d202ab6ab1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:58Z</t>
+  </si>
+  <si>
+    <t>20c420f5dbb975062c4a39ffaf73b319</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.acd5b7d6f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T08:59:59Z</t>
+  </si>
+  <si>
+    <t>a57cb95b02968070e4838c495521082f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.0b9c0841c8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>cfea79377513817fa515ae42eca7fd0a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.3a0babcede^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T09:00:00Z</t>
+  </si>
+  <si>
+    <t>ea8b199f47e837b2c86494d02e6fc8ac</t>
+  </si>
+  <si>
+    <t>2026-01-30T09:00:01Z</t>
+  </si>
+  <si>
+    <t>8f4b79b31d0d974fc030f69c200aec23</t>
+  </si>
+  <si>
+    <t>f00a53fb770f32cd8b8a6cdb0a5f4065</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.c187be9952^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T09:00:02Z</t>
+  </si>
+  <si>
+    <t>2026-01-30T09:00:03Z</t>
+  </si>
+  <si>
+    <t>6f2e64d7c1a3a89805aeb76d5461e189</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.b4252c868b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T09:00:04Z</t>
+  </si>
+  <si>
+    <t>219249d6ee23684533d7ad6f386e744e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.b55ea5baca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-01-30T09:00:05Z</t>
+  </si>
+  <si>
+    <t>6b8ac44590f1d4f1415a17382ffcc9e2</t>
+  </si>
+  <si>
+    <t>6506aa66-1c27-4e22-abcc-e215717942f0.9c717939a2a9a31bd0fab64231e9b14ca6e2d16958b3a06f57f0701c867c9b72.021bb4461a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4020,10 +4035,10 @@
   <dimension ref="A1:W750"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A184" sqref="A184:XFD184"/>
+      <selection pane="bottomRight" activeCell="I193" sqref="I193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4070,7 +4085,7 @@
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="55" t="s">
-        <v>498</v>
+        <v>446</v>
       </c>
       <c r="D2" s="54"/>
       <c r="F2" s="6"/>
@@ -4438,16 +4453,16 @@
         <v>43</v>
       </c>
       <c r="F13" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="H13" s="48" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>493</v>
+        <v>444</v>
       </c>
       <c r="J13" s="38" t="s">
         <v>64</v>
@@ -4461,7 +4476,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P13" s="50" t="s">
         <v>64</v>
@@ -4473,7 +4488,7 @@
         <v>64</v>
       </c>
       <c r="S13" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T13" s="38"/>
       <c r="U13" s="39"/>
@@ -4758,16 +4773,16 @@
         <v>55</v>
       </c>
       <c r="F21" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G21" s="48" t="s">
+        <v>490</v>
+      </c>
+      <c r="H21" s="48" t="s">
         <v>491</v>
       </c>
-      <c r="H21" s="48" t="s">
-        <v>492</v>
-      </c>
       <c r="I21" s="48" t="s">
-        <v>493</v>
+        <v>444</v>
       </c>
       <c r="J21" s="38" t="s">
         <v>64</v>
@@ -4781,7 +4796,7 @@
         <v>64</v>
       </c>
       <c r="O21" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P21" s="50" t="s">
         <v>64</v>
@@ -4793,7 +4808,7 @@
         <v>64</v>
       </c>
       <c r="S21" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T21" s="38"/>
       <c r="U21" s="39"/>
@@ -5082,10 +5097,10 @@
         <v>425</v>
       </c>
       <c r="F29" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G29" s="48" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="H29" s="37"/>
       <c r="I29" s="42"/>
@@ -5101,7 +5116,7 @@
         <v>64</v>
       </c>
       <c r="O29" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P29" s="50" t="s">
         <v>64</v>
@@ -5113,7 +5128,7 @@
         <v>64</v>
       </c>
       <c r="S29" s="50" t="s">
-        <v>496</v>
+        <v>445</v>
       </c>
       <c r="T29" s="38"/>
       <c r="U29" s="39" t="s">
@@ -8888,16 +8903,16 @@
         <v>333</v>
       </c>
       <c r="F131" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G131" s="48" t="s">
-        <v>487</v>
+        <v>447</v>
       </c>
       <c r="H131" s="48" t="s">
-        <v>488</v>
+        <v>448</v>
       </c>
       <c r="I131" s="48" t="s">
-        <v>489</v>
+        <v>449</v>
       </c>
       <c r="J131" s="38" t="s">
         <v>64</v>
@@ -8911,7 +8926,7 @@
         <v>64</v>
       </c>
       <c r="O131" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P131" s="50" t="s">
         <v>64</v>
@@ -8923,7 +8938,7 @@
         <v>64</v>
       </c>
       <c r="S131" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T131" s="38"/>
       <c r="U131" s="39"/>
@@ -8949,16 +8964,16 @@
         <v>334</v>
       </c>
       <c r="F132" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G132" s="48" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="H132" s="48" t="s">
-        <v>485</v>
+        <v>451</v>
       </c>
       <c r="I132" s="48" t="s">
-        <v>486</v>
+        <v>452</v>
       </c>
       <c r="J132" s="38" t="s">
         <v>64</v>
@@ -8972,7 +8987,7 @@
         <v>64</v>
       </c>
       <c r="O132" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P132" s="50" t="s">
         <v>64</v>
@@ -8984,7 +8999,7 @@
         <v>64</v>
       </c>
       <c r="S132" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T132" s="38"/>
       <c r="U132" s="39"/>
@@ -9010,16 +9025,16 @@
         <v>335</v>
       </c>
       <c r="F133" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G133" s="48" t="s">
-        <v>481</v>
+        <v>450</v>
       </c>
       <c r="H133" s="48" t="s">
-        <v>482</v>
+        <v>453</v>
       </c>
       <c r="I133" s="48" t="s">
-        <v>483</v>
+        <v>454</v>
       </c>
       <c r="J133" s="38" t="s">
         <v>64</v>
@@ -9033,7 +9048,7 @@
         <v>64</v>
       </c>
       <c r="O133" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P133" s="50" t="s">
         <v>64</v>
@@ -9045,7 +9060,7 @@
         <v>64</v>
       </c>
       <c r="S133" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T133" s="38"/>
       <c r="U133" s="39"/>
@@ -9071,16 +9086,16 @@
         <v>336</v>
       </c>
       <c r="F134" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G134" s="48" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="H134" s="48" t="s">
-        <v>479</v>
+        <v>457</v>
       </c>
       <c r="I134" s="48" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="J134" s="38" t="s">
         <v>64</v>
@@ -9094,7 +9109,7 @@
         <v>64</v>
       </c>
       <c r="O134" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P134" s="50" t="s">
         <v>64</v>
@@ -9106,7 +9121,7 @@
         <v>64</v>
       </c>
       <c r="S134" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T134" s="38"/>
       <c r="U134" s="39"/>
@@ -9132,16 +9147,16 @@
         <v>337</v>
       </c>
       <c r="F135" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G135" s="48" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="H135" s="48" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="I135" s="48" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="J135" s="38" t="s">
         <v>64</v>
@@ -9155,7 +9170,7 @@
         <v>64</v>
       </c>
       <c r="O135" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P135" s="50" t="s">
         <v>64</v>
@@ -9167,7 +9182,7 @@
         <v>64</v>
       </c>
       <c r="S135" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T135" s="38"/>
       <c r="U135" s="39"/>
@@ -9193,16 +9208,16 @@
         <v>206</v>
       </c>
       <c r="F136" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G136" s="48" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="H136" s="48" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="I136" s="48" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="J136" s="38" t="s">
         <v>64</v>
@@ -9216,7 +9231,7 @@
         <v>64</v>
       </c>
       <c r="O136" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P136" s="50" t="s">
         <v>64</v>
@@ -9228,7 +9243,7 @@
         <v>64</v>
       </c>
       <c r="S136" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T136" s="38"/>
       <c r="U136" s="39"/>
@@ -9254,16 +9269,16 @@
         <v>338</v>
       </c>
       <c r="F137" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G137" s="48" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="H137" s="48" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="I137" s="48" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="J137" s="38" t="s">
         <v>64</v>
@@ -9277,7 +9292,7 @@
         <v>64</v>
       </c>
       <c r="O137" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P137" s="50" t="s">
         <v>64</v>
@@ -9289,7 +9304,7 @@
         <v>64</v>
       </c>
       <c r="S137" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T137" s="38"/>
       <c r="U137" s="39"/>
@@ -9315,16 +9330,16 @@
         <v>339</v>
       </c>
       <c r="F138" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G138" s="48" t="s">
+        <v>466</v>
+      </c>
+      <c r="H138" s="48" t="s">
         <v>467</v>
       </c>
-      <c r="H138" s="48" t="s">
+      <c r="I138" s="48" t="s">
         <v>468</v>
-      </c>
-      <c r="I138" s="48" t="s">
-        <v>469</v>
       </c>
       <c r="J138" s="38" t="s">
         <v>64</v>
@@ -9338,7 +9353,7 @@
         <v>64</v>
       </c>
       <c r="O138" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P138" s="50" t="s">
         <v>64</v>
@@ -9350,7 +9365,7 @@
         <v>64</v>
       </c>
       <c r="S138" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T138" s="38"/>
       <c r="U138" s="39"/>
@@ -9376,16 +9391,16 @@
         <v>340</v>
       </c>
       <c r="F139" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G139" s="48" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="H139" s="48" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="I139" s="48" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="J139" s="38" t="s">
         <v>64</v>
@@ -9399,7 +9414,7 @@
         <v>64</v>
       </c>
       <c r="O139" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P139" s="50" t="s">
         <v>64</v>
@@ -9411,7 +9426,7 @@
         <v>64</v>
       </c>
       <c r="S139" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T139" s="38"/>
       <c r="U139" s="39"/>
@@ -9437,16 +9452,16 @@
         <v>341</v>
       </c>
       <c r="F140" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G140" s="48" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
       <c r="H140" s="48" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="I140" s="48" t="s">
-        <v>463</v>
+        <v>474</v>
       </c>
       <c r="J140" s="38" t="s">
         <v>64</v>
@@ -9460,7 +9475,7 @@
         <v>64</v>
       </c>
       <c r="O140" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P140" s="50" t="s">
         <v>64</v>
@@ -9472,7 +9487,7 @@
         <v>64</v>
       </c>
       <c r="S140" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T140" s="38"/>
       <c r="U140" s="39"/>
@@ -9498,16 +9513,16 @@
         <v>342</v>
       </c>
       <c r="F141" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G141" s="48" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="H141" s="48" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="I141" s="48" t="s">
-        <v>460</v>
+        <v>476</v>
       </c>
       <c r="J141" s="38" t="s">
         <v>64</v>
@@ -9521,7 +9536,7 @@
         <v>64</v>
       </c>
       <c r="O141" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P141" s="50" t="s">
         <v>64</v>
@@ -9533,7 +9548,7 @@
         <v>64</v>
       </c>
       <c r="S141" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T141" s="38"/>
       <c r="U141" s="39"/>
@@ -9558,17 +9573,17 @@
       <c r="E142" s="43" t="s">
         <v>343</v>
       </c>
-      <c r="F142" s="37">
-        <v>45484</v>
+      <c r="F142" s="47">
+        <v>46052</v>
       </c>
       <c r="G142" s="48" t="s">
-        <v>455</v>
+        <v>477</v>
       </c>
       <c r="H142" s="48" t="s">
-        <v>456</v>
+        <v>478</v>
       </c>
       <c r="I142" s="48" t="s">
-        <v>457</v>
+        <v>479</v>
       </c>
       <c r="J142" s="38" t="s">
         <v>64</v>
@@ -9582,7 +9597,7 @@
         <v>64</v>
       </c>
       <c r="O142" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P142" s="50" t="s">
         <v>64</v>
@@ -9594,7 +9609,7 @@
         <v>64</v>
       </c>
       <c r="S142" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T142" s="38"/>
       <c r="U142" s="39"/>
@@ -9620,16 +9635,16 @@
         <v>344</v>
       </c>
       <c r="F143" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G143" s="48" t="s">
-        <v>452</v>
+        <v>480</v>
       </c>
       <c r="H143" s="48" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="I143" s="48" t="s">
-        <v>454</v>
+        <v>482</v>
       </c>
       <c r="J143" s="38" t="s">
         <v>64</v>
@@ -9643,7 +9658,7 @@
         <v>64</v>
       </c>
       <c r="O143" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P143" s="50" t="s">
         <v>64</v>
@@ -9655,7 +9670,7 @@
         <v>64</v>
       </c>
       <c r="S143" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T143" s="38"/>
       <c r="U143" s="39"/>
@@ -9681,16 +9696,16 @@
         <v>345</v>
       </c>
       <c r="F144" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G144" s="48" t="s">
-        <v>445</v>
+        <v>483</v>
       </c>
       <c r="H144" s="48" t="s">
-        <v>450</v>
+        <v>484</v>
       </c>
       <c r="I144" s="48" t="s">
-        <v>451</v>
+        <v>485</v>
       </c>
       <c r="J144" s="38" t="s">
         <v>64</v>
@@ -9704,7 +9719,7 @@
         <v>64</v>
       </c>
       <c r="O144" s="50" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P144" s="50" t="s">
         <v>64</v>
@@ -9716,7 +9731,7 @@
         <v>64</v>
       </c>
       <c r="S144" s="50" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T144" s="38"/>
       <c r="U144" s="39"/>
@@ -9742,16 +9757,16 @@
         <v>346</v>
       </c>
       <c r="F145" s="47">
-        <v>45484</v>
+        <v>46052</v>
       </c>
       <c r="G145" s="48" t="s">
-        <v>445</v>
-      </c>
-      <c r="H145" s="48" t="s">
-        <v>446</v>
+        <v>483</v>
+      </c>
+      <c r="H145" s="37" t="s">
+        <v>486</v>
       </c>
       <c r="I145" s="48" t="s">
-        <v>447</v>
+        <v>487</v>
       </c>
       <c r="J145" s="38" t="s">
         <v>64</v>
@@ -9765,7 +9780,7 @@
         <v>64</v>
       </c>
       <c r="O145" s="49" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="P145" s="38" t="s">
         <v>64</v>
@@ -9777,7 +9792,7 @@
         <v>64</v>
       </c>
       <c r="S145" s="49" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="T145" s="38"/>
       <c r="U145" s="39"/>
@@ -10914,7 +10929,7 @@
       </c>
       <c r="F176" s="35"/>
       <c r="G176" s="35"/>
-      <c r="H176" s="35"/>
+      <c r="H176" s="37"/>
       <c r="I176" s="35"/>
       <c r="J176" s="38"/>
       <c r="K176" s="38"/>
@@ -10951,7 +10966,7 @@
       </c>
       <c r="F177" s="35"/>
       <c r="G177" s="35"/>
-      <c r="H177" s="35"/>
+      <c r="H177" s="37"/>
       <c r="I177" s="35"/>
       <c r="J177" s="38"/>
       <c r="K177" s="38"/>
@@ -10988,7 +11003,7 @@
       </c>
       <c r="F178" s="35"/>
       <c r="G178" s="35"/>
-      <c r="H178" s="35"/>
+      <c r="H178" s="37"/>
       <c r="I178" s="35"/>
       <c r="J178" s="38"/>
       <c r="K178" s="38"/>
@@ -11025,7 +11040,7 @@
       </c>
       <c r="F179" s="35"/>
       <c r="G179" s="35"/>
-      <c r="H179" s="35"/>
+      <c r="H179" s="37"/>
       <c r="I179" s="35"/>
       <c r="J179" s="38"/>
       <c r="K179" s="38"/>
@@ -11062,7 +11077,7 @@
       </c>
       <c r="F180" s="35"/>
       <c r="G180" s="35"/>
-      <c r="H180" s="35"/>
+      <c r="H180" s="37"/>
       <c r="I180" s="35"/>
       <c r="J180" s="38"/>
       <c r="K180" s="38"/>
@@ -11099,7 +11114,7 @@
       </c>
       <c r="F181" s="35"/>
       <c r="G181" s="35"/>
-      <c r="H181" s="35"/>
+      <c r="H181" s="37"/>
       <c r="I181" s="35"/>
       <c r="J181" s="38"/>
       <c r="K181" s="38"/>
@@ -11136,7 +11151,7 @@
       </c>
       <c r="F182" s="35"/>
       <c r="G182" s="35"/>
-      <c r="H182" s="35"/>
+      <c r="H182" s="37"/>
       <c r="I182" s="35"/>
       <c r="J182" s="38"/>
       <c r="K182" s="38"/>
@@ -11173,7 +11188,7 @@
       </c>
       <c r="F183" s="35"/>
       <c r="G183" s="35"/>
-      <c r="H183" s="35"/>
+      <c r="H183" s="37"/>
       <c r="I183" s="35"/>
       <c r="J183" s="38"/>
       <c r="K183" s="38"/>
@@ -11208,26 +11223,44 @@
       <c r="E184" s="43" t="s">
         <v>398</v>
       </c>
-      <c r="F184" s="35"/>
-      <c r="G184" s="35"/>
-      <c r="H184" s="35"/>
-      <c r="I184" s="35"/>
+      <c r="F184" s="47">
+        <v>46052</v>
+      </c>
+      <c r="G184" s="35" t="s">
+        <v>490</v>
+      </c>
+      <c r="H184" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="I184" s="48" t="s">
+        <v>493</v>
+      </c>
       <c r="J184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K184" s="38"/>
+      <c r="L184" s="38"/>
+      <c r="M184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O184" s="49" t="s">
+        <v>442</v>
+      </c>
+      <c r="P184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q184" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="K184" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="L184" s="38" t="s">
-        <v>497</v>
-      </c>
-      <c r="M184" s="38"/>
-      <c r="N184" s="38"/>
-      <c r="O184" s="35"/>
-      <c r="P184" s="38"/>
-      <c r="Q184" s="38"/>
-      <c r="R184" s="38"/>
-      <c r="S184" s="35"/>
+      <c r="R184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S184" s="49" t="s">
+        <v>443</v>
+      </c>
       <c r="T184" s="38"/>
       <c r="U184" s="35"/>
       <c r="V184" s="35"/>
@@ -11473,19 +11506,23 @@
       <c r="E191" s="43" t="s">
         <v>433</v>
       </c>
-      <c r="F191" s="37"/>
-      <c r="G191" s="37"/>
-      <c r="H191" s="37"/>
-      <c r="I191" s="42"/>
+      <c r="F191" s="47">
+        <v>46052</v>
+      </c>
+      <c r="G191" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="H191" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="I191" s="42" t="s">
+        <v>497</v>
+      </c>
       <c r="J191" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="K191" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="L191" s="38" t="s">
-        <v>497</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="K191" s="38"/>
+      <c r="L191" s="38"/>
       <c r="M191" s="38"/>
       <c r="N191" s="38"/>
       <c r="O191" s="38"/>
@@ -11516,19 +11553,23 @@
       <c r="E192" s="43" t="s">
         <v>434</v>
       </c>
-      <c r="F192" s="37"/>
-      <c r="G192" s="37"/>
-      <c r="H192" s="37"/>
-      <c r="I192" s="42"/>
+      <c r="F192" s="47">
+        <v>46052</v>
+      </c>
+      <c r="G192" s="37" t="s">
+        <v>498</v>
+      </c>
+      <c r="H192" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="I192" s="42" t="s">
+        <v>500</v>
+      </c>
       <c r="J192" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="K192" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="L192" s="38" t="s">
-        <v>497</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="K192" s="38"/>
+      <c r="L192" s="38"/>
       <c r="M192" s="38"/>
       <c r="N192" s="38"/>
       <c r="O192" s="38"/>
@@ -11559,17 +11600,17 @@
       <c r="E193" s="45" t="s">
         <v>437</v>
       </c>
-      <c r="F193" s="37">
-        <v>45996</v>
+      <c r="F193" s="47">
+        <v>46052</v>
       </c>
       <c r="G193" s="37" t="s">
-        <v>442</v>
+        <v>501</v>
       </c>
       <c r="H193" s="37" t="s">
-        <v>443</v>
+        <v>502</v>
       </c>
       <c r="I193" s="42" t="s">
-        <v>444</v>
+        <v>503</v>
       </c>
       <c r="J193" s="38" t="s">
         <v>64</v>
@@ -17837,6 +17878,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -17980,12 +18027,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -17996,6 +18037,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18013,23 +18071,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Aggiornati test 476 e 477
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#ADLINGEGNERIAINFORMATICAXX/ADL/ARIA/2.99.2/report-checklist.xlsx
+++ b/GATEWAY/A1#111#ADLINGEGNERIAINFORMATICAXX/ADL/ARIA/2.99.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\ACCREDITAMENTO\it-fse-accreditamento\GATEWAY\A1#111#ADLINGEGNERIAINFORMATICAXX\ADL\ARIA\2.99.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCC6E0F-EFB5-412A-9E53-246AEDCDD059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F72B02-13C9-457D-A9DE-571E9DEAABA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1896,24 +1896,6 @@
     <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.080f5abeb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2026-02-06T11:01:55Z</t>
-  </si>
-  <si>
-    <t>3dcfef578c0eff84d6e67a03ed9614b8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.6f28ade170^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2026-02-06T11:01:56Z</t>
-  </si>
-  <si>
-    <t>dd1c475ff37a5ab38bb7912cf8ab8a2c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.40bacba66d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2026-02-06T11:01:57Z</t>
   </si>
   <si>
@@ -1921,6 +1903,24 @@
   </si>
   <si>
     <t>6506aa66-1c27-4e22-abcc-e215717942f0.9c717939a2a9a31bd0fab64231e9b14ca6e2d16958b3a06f57f0701c867c9b72.a0cad8a039^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-02-12T13:57:42Z</t>
+  </si>
+  <si>
+    <t>8c443979be9199f44aa7c555d7647dd1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.569e03155d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2026-02-12T13:57:44Z</t>
+  </si>
+  <si>
+    <t>16d9564abba1c2a40e8ca8ea7aac9c38</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.50.2.12345.4.4.2.d44d586b8d0bfc6960cb68deb8efc3e746a94a6d211f4ee356d8cefda8dbb66a.35bd66dac6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4050,7 +4050,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="E145" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I193" sqref="I193"/>
+      <selection pane="bottomRight" activeCell="I192" sqref="I192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11519,16 +11519,16 @@
         <v>433</v>
       </c>
       <c r="F191" s="47">
-        <v>46059</v>
+        <v>46065</v>
       </c>
       <c r="G191" s="37" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="H191" s="37" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="I191" s="42" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="J191" s="38" t="s">
         <v>64</v>
@@ -11566,16 +11566,16 @@
         <v>434</v>
       </c>
       <c r="F192" s="47">
-        <v>46059</v>
+        <v>46065</v>
       </c>
       <c r="G192" s="37" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="H192" s="37" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="J192" s="38" t="s">
         <v>64</v>
@@ -11616,13 +11616,13 @@
         <v>46059</v>
       </c>
       <c r="G193" s="37" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="H193" s="37" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="I193" s="42" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="J193" s="38" t="s">
         <v>64</v>
@@ -17890,15 +17890,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BE9A258ADBC3EC4CBEB1E2AB9909207A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0284f501378927579289f00316ec8a74">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="295b7897-c886-40bf-9750-5782b814c3e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b47213d65be806e283915cff374a7eef" ns2:_="">
     <xsd:import namespace="295b7897-c886-40bf-9750-5782b814c3e4"/>
@@ -18042,6 +18033,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -18049,14 +18049,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7568E770-0BC4-46AF-B6C6-958AE21C8F7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18070,6 +18062,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>